<commit_message>
NB Reporting: - KZT Form 8 done (IFRS-9)
</commit_message>
<xml_diff>
--- a/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_8.xlsx
+++ b/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_8.xlsx
@@ -18,7 +18,7 @@
     <definedName name="GR_CODE_ROW">4583</definedName>
     <definedName name="GR_CODE_SHEET">4</definedName>
     <definedName name="_xlnm.Database">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">РТПДЗ_8!$A$1:$R$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">РТПДЗ_8!$A$1:$R$34</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Код формы</t>
   </si>
@@ -134,21 +134,9 @@
  дней</t>
   </si>
   <si>
-    <t>Краткосрочная торговая и прочая дебиторская задолженность (сумма строк 2-9)</t>
-  </si>
-  <si>
     <t>Краткосрочная дебиторская задолженность покупателей и заказчиков</t>
   </si>
   <si>
-    <t>Краткосрочная дебиторская задолженность дочерних организаций</t>
-  </si>
-  <si>
-    <t>Краткосрочная дебиторская задолженность ассоциированных и совместных организаций</t>
-  </si>
-  <si>
-    <t>Краткосрочная дебиторская задолженность филиалов и представительств</t>
-  </si>
-  <si>
     <t>Краткосрочная дебиторская задолженность работников</t>
   </si>
   <si>
@@ -161,21 +149,9 @@
     <t>Прочая краткосрочная дебиторская задолженность</t>
   </si>
   <si>
-    <t>Долгосрочная торговая и прочая дебиторская задолженность (сумма строк 11-18)</t>
-  </si>
-  <si>
     <t>Долгосрочная задолженность покупателей и заказчиков</t>
   </si>
   <si>
-    <t>Долгосрочная дебиторская задолженность дочерних организаций</t>
-  </si>
-  <si>
-    <t>Долгосрочная дебиторская задолженность ассоциированных и совместных организаций</t>
-  </si>
-  <si>
-    <t>Долгосрочная дебиторская задолженность филиалов и представительств</t>
-  </si>
-  <si>
     <t>Долгосрочная дебиторская задолженность работников</t>
   </si>
   <si>
@@ -188,9 +164,6 @@
     <t>Прочая долгосрочная дебиторская задолженность</t>
   </si>
   <si>
-    <t>ВСЕГО (сумма строк 1, 10)</t>
-  </si>
-  <si>
     <t>* В гр.1 четвертый знак номера счета указывается с учетом принадлежности к контрагентам (эмитентам), то есть от 1 до 3</t>
   </si>
   <si>
@@ -210,6 +183,15 @@
   </si>
   <si>
     <t>&lt;dd.MM.yyyy&gt;</t>
+  </si>
+  <si>
+    <t>Краткосрочная торговая и прочая дебиторская задолженность (сумма строк 2-6)</t>
+  </si>
+  <si>
+    <t>Долгосрочная торговая и прочая дебиторская задолженность (сумма строк 8-12)</t>
+  </si>
+  <si>
+    <t>Всего (сумма строк 1, 7)</t>
   </si>
 </sst>
 </file>
@@ -468,7 +450,7 @@
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -533,9 +515,6 @@
     <xf numFmtId="16" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -595,70 +574,6 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -671,8 +586,69 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="27">
@@ -1017,10 +993,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:R46"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2144,8 +2120,8 @@
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="51" t="s">
-        <v>57</v>
+      <c r="C2" s="50" t="s">
+        <v>48</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -2290,48 +2266,48 @@
       <c r="R8" s="6"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="53"/>
-      <c r="M9" s="53"/>
-      <c r="N9" s="53"/>
-      <c r="O9" s="53"/>
-      <c r="P9" s="53"/>
-      <c r="Q9" s="53"/>
-      <c r="R9" s="53"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="58"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="58"/>
+      <c r="Q9" s="58"/>
+      <c r="R9" s="58"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="53"/>
-      <c r="P10" s="53"/>
-      <c r="Q10" s="53"/>
-      <c r="R10" s="53"/>
+      <c r="A10" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="58"/>
+      <c r="O10" s="58"/>
+      <c r="P10" s="58"/>
+      <c r="Q10" s="58"/>
+      <c r="R10" s="58"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D11" s="3"/>
@@ -2368,92 +2344,92 @@
       <c r="R12" s="3"/>
     </row>
     <row r="13" spans="1:18" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="57" t="s">
+      <c r="C13" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="58" t="s">
+      <c r="D13" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="59"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="57" t="s">
+      <c r="E13" s="64"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="57" t="s">
+      <c r="H13" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="I13" s="61" t="s">
+      <c r="I13" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="61"/>
-      <c r="K13" s="61"/>
-      <c r="L13" s="61"/>
-      <c r="M13" s="62" t="s">
+      <c r="J13" s="66"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="N13" s="62"/>
-      <c r="O13" s="62"/>
-      <c r="P13" s="62"/>
-      <c r="Q13" s="67" t="s">
+      <c r="N13" s="67"/>
+      <c r="O13" s="67"/>
+      <c r="P13" s="67"/>
+      <c r="Q13" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="R13" s="67" t="s">
+      <c r="R13" s="72" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:18" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="55"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="54" t="s">
+      <c r="A14" s="60"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="54" t="s">
+      <c r="E14" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="54" t="s">
+      <c r="F14" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="70" t="s">
+      <c r="G14" s="62"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="71"/>
-      <c r="K14" s="72"/>
-      <c r="L14" s="54" t="s">
+      <c r="J14" s="76"/>
+      <c r="K14" s="77"/>
+      <c r="L14" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="M14" s="52" t="s">
+      <c r="M14" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="N14" s="52" t="s">
+      <c r="N14" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="O14" s="52" t="s">
+      <c r="O14" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="P14" s="52" t="s">
+      <c r="P14" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="Q14" s="68"/>
-      <c r="R14" s="68"/>
+      <c r="Q14" s="73"/>
+      <c r="R14" s="73"/>
     </row>
     <row r="15" spans="1:18" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="56"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
+      <c r="A15" s="61"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
       <c r="I15" s="13" t="s">
         <v>29</v>
       </c>
@@ -2463,13 +2439,13 @@
       <c r="K15" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="L15" s="56"/>
-      <c r="M15" s="52"/>
-      <c r="N15" s="52"/>
-      <c r="O15" s="52"/>
-      <c r="P15" s="52"/>
-      <c r="Q15" s="69"/>
-      <c r="R15" s="69"/>
+      <c r="L15" s="61"/>
+      <c r="M15" s="57"/>
+      <c r="N15" s="57"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="57"/>
+      <c r="Q15" s="74"/>
+      <c r="R15" s="74"/>
     </row>
     <row r="16" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
@@ -2530,38 +2506,38 @@
     <row r="17" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" s="18" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C17" s="19">
         <v>1</v>
       </c>
-      <c r="D17" s="73"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="74"/>
-      <c r="K17" s="74"/>
-      <c r="L17" s="74"/>
-      <c r="M17" s="75"/>
-      <c r="N17" s="75"/>
-      <c r="O17" s="75"/>
-      <c r="P17" s="75"/>
-      <c r="Q17" s="73"/>
-      <c r="R17" s="73"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="53"/>
+      <c r="P17" s="53"/>
+      <c r="Q17" s="51"/>
+      <c r="R17" s="51"/>
     </row>
     <row r="18" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="23">
         <v>2</v>
       </c>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="20"/>
@@ -2572,20 +2548,20 @@
       <c r="N18" s="21"/>
       <c r="O18" s="21"/>
       <c r="P18" s="21"/>
-      <c r="Q18" s="46"/>
-      <c r="R18" s="46"/>
-    </row>
-    <row r="19" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q18" s="45"/>
+      <c r="R18" s="45"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
       <c r="B19" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="23">
         <v>3</v>
       </c>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
       <c r="I19" s="20"/>
@@ -2596,20 +2572,20 @@
       <c r="N19" s="21"/>
       <c r="O19" s="21"/>
       <c r="P19" s="21"/>
-      <c r="Q19" s="46"/>
-      <c r="R19" s="46"/>
-    </row>
-    <row r="20" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q19" s="45"/>
+      <c r="R19" s="45"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
       <c r="B20" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="23">
         <v>4</v>
       </c>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
       <c r="I20" s="20"/>
@@ -2620,13 +2596,13 @@
       <c r="N20" s="21"/>
       <c r="O20" s="21"/>
       <c r="P20" s="21"/>
-      <c r="Q20" s="46"/>
-      <c r="R20" s="46"/>
-    </row>
-    <row r="21" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
+      <c r="Q20" s="45"/>
+      <c r="R20" s="45"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
       <c r="B21" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="23">
         <v>5</v>
@@ -2634,12 +2610,12 @@
       <c r="D21" s="48"/>
       <c r="E21" s="48"/>
       <c r="F21" s="48"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
       <c r="M21" s="21"/>
       <c r="N21" s="21"/>
       <c r="O21" s="21"/>
@@ -2648,40 +2624,40 @@
       <c r="R21" s="46"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="23">
+      <c r="A22" s="24"/>
+      <c r="B22" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="19">
         <v>6</v>
       </c>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
       <c r="F22" s="48"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="46"/>
-      <c r="R22" s="46"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="53"/>
+      <c r="N22" s="53"/>
+      <c r="O22" s="53"/>
+      <c r="P22" s="53"/>
+      <c r="Q22" s="55"/>
+      <c r="R22" s="55"/>
+    </row>
+    <row r="23" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
-      <c r="B23" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="23">
+      <c r="B23" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="19">
         <v>7</v>
       </c>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
       <c r="I23" s="20"/>
@@ -2692,68 +2668,68 @@
       <c r="N23" s="21"/>
       <c r="O23" s="21"/>
       <c r="P23" s="21"/>
-      <c r="Q23" s="46"/>
+      <c r="Q23" s="45"/>
       <c r="R23" s="46"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="25">
+        <v>37</v>
+      </c>
+      <c r="C24" s="23">
         <v>8</v>
       </c>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
       <c r="M24" s="21"/>
       <c r="N24" s="21"/>
       <c r="O24" s="21"/>
       <c r="P24" s="21"/>
-      <c r="Q24" s="47"/>
-      <c r="R24" s="47"/>
+      <c r="Q24" s="45"/>
+      <c r="R24" s="45"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="78" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="79">
+      <c r="A25" s="17"/>
+      <c r="B25" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="23">
         <v>9</v>
       </c>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="76"/>
-      <c r="H25" s="76"/>
-      <c r="I25" s="76"/>
-      <c r="J25" s="76"/>
-      <c r="K25" s="76"/>
-      <c r="L25" s="76"/>
-      <c r="M25" s="75"/>
-      <c r="N25" s="75"/>
-      <c r="O25" s="75"/>
-      <c r="P25" s="75"/>
-      <c r="Q25" s="77"/>
-      <c r="R25" s="77"/>
-    </row>
-    <row r="26" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="45"/>
+      <c r="R25" s="45"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
-      <c r="B26" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="19">
+      <c r="B26" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="23">
         <v>10</v>
       </c>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
       <c r="I26" s="20"/>
@@ -2764,20 +2740,20 @@
       <c r="N26" s="21"/>
       <c r="O26" s="21"/>
       <c r="P26" s="21"/>
-      <c r="Q26" s="46"/>
-      <c r="R26" s="47"/>
+      <c r="Q26" s="45"/>
+      <c r="R26" s="45"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C27" s="23">
         <v>11</v>
       </c>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
@@ -2788,20 +2764,20 @@
       <c r="N27" s="21"/>
       <c r="O27" s="21"/>
       <c r="P27" s="21"/>
-      <c r="Q27" s="46"/>
-      <c r="R27" s="46"/>
-    </row>
-    <row r="28" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q27" s="45"/>
+      <c r="R27" s="45"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
       <c r="B28" s="22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C28" s="23">
         <v>12</v>
       </c>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
       <c r="I28" s="20"/>
@@ -2812,365 +2788,221 @@
       <c r="N28" s="21"/>
       <c r="O28" s="21"/>
       <c r="P28" s="21"/>
-      <c r="Q28" s="46"/>
-      <c r="R28" s="46"/>
-    </row>
-    <row r="29" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="22" t="s">
+      <c r="Q28" s="45"/>
+      <c r="R28" s="45"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="69" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="70"/>
+      <c r="C29" s="27">
+        <v>13</v>
+      </c>
+      <c r="D29" s="55"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="54"/>
+      <c r="K29" s="54"/>
+      <c r="L29" s="54"/>
+      <c r="M29" s="53"/>
+      <c r="N29" s="53"/>
+      <c r="O29" s="53"/>
+      <c r="P29" s="53"/>
+      <c r="Q29" s="51"/>
+      <c r="R29" s="55"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="28"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="31"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="31"/>
+      <c r="P30" s="31"/>
+      <c r="Q30" s="31"/>
+      <c r="R30" s="31"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B31" s="71" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="71"/>
+      <c r="D31" s="71"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="71"/>
+      <c r="G31" s="71"/>
+      <c r="H31" s="71"/>
+      <c r="I31" s="71"/>
+      <c r="J31" s="71"/>
+      <c r="K31" s="71"/>
+      <c r="L31" s="71"/>
+      <c r="M31" s="71"/>
+      <c r="N31" s="71"/>
+      <c r="O31" s="71"/>
+      <c r="P31" s="71"/>
+      <c r="Q31" s="71"/>
+      <c r="R31" s="71"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="32"/>
+      <c r="B32" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="71"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="71"/>
+      <c r="J32" s="71"/>
+      <c r="K32" s="71"/>
+      <c r="L32" s="71"/>
+      <c r="M32" s="71"/>
+      <c r="N32" s="71"/>
+      <c r="O32" s="71"/>
+      <c r="P32" s="71"/>
+      <c r="Q32" s="71"/>
+      <c r="R32" s="71"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="32"/>
+      <c r="B33" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="23">
-        <v>13</v>
-      </c>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="21"/>
-      <c r="Q29" s="46"/>
-      <c r="R29" s="46"/>
-    </row>
-    <row r="30" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="22" t="s">
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="71"/>
+      <c r="I33" s="71"/>
+      <c r="J33" s="71"/>
+      <c r="K33" s="71"/>
+      <c r="L33" s="71"/>
+      <c r="M33" s="71"/>
+      <c r="N33" s="71"/>
+      <c r="O33" s="71"/>
+      <c r="P33" s="71"/>
+      <c r="Q33" s="71"/>
+      <c r="R33" s="71"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="32"/>
+      <c r="B34" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="23">
-        <v>14</v>
-      </c>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="21"/>
-      <c r="N30" s="21"/>
-      <c r="O30" s="21"/>
-      <c r="P30" s="21"/>
-      <c r="Q30" s="46"/>
-      <c r="R30" s="46"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="22" t="s">
+      <c r="C34" s="71"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="71"/>
+      <c r="I34" s="71"/>
+      <c r="J34" s="71"/>
+      <c r="K34" s="71"/>
+      <c r="L34" s="71"/>
+      <c r="M34" s="71"/>
+      <c r="N34" s="71"/>
+      <c r="O34" s="71"/>
+      <c r="P34" s="71"/>
+      <c r="Q34" s="71"/>
+      <c r="R34" s="71"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="32"/>
+      <c r="B35" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="23">
-        <v>15</v>
-      </c>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
-      <c r="O31" s="21"/>
-      <c r="P31" s="21"/>
-      <c r="Q31" s="46"/>
-      <c r="R31" s="46"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" s="23">
-        <v>16</v>
-      </c>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="21"/>
-      <c r="N32" s="21"/>
-      <c r="O32" s="21"/>
-      <c r="P32" s="21"/>
-      <c r="Q32" s="46"/>
-      <c r="R32" s="46"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-      <c r="B33" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C33" s="23">
-        <v>17</v>
-      </c>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
-      <c r="M33" s="21"/>
-      <c r="N33" s="21"/>
-      <c r="O33" s="21"/>
-      <c r="P33" s="21"/>
-      <c r="Q33" s="46"/>
-      <c r="R33" s="46"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
-      <c r="B34" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="23">
-        <v>18</v>
-      </c>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="21"/>
-      <c r="N34" s="21"/>
-      <c r="O34" s="21"/>
-      <c r="P34" s="21"/>
-      <c r="Q34" s="46"/>
-      <c r="R34" s="46"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="64" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35" s="65"/>
-      <c r="C35" s="28">
-        <v>19</v>
-      </c>
-      <c r="D35" s="77"/>
-      <c r="E35" s="73"/>
-      <c r="F35" s="77"/>
-      <c r="G35" s="76"/>
-      <c r="H35" s="76"/>
-      <c r="I35" s="76"/>
-      <c r="J35" s="76"/>
-      <c r="K35" s="76"/>
-      <c r="L35" s="76"/>
-      <c r="M35" s="75"/>
-      <c r="N35" s="75"/>
-      <c r="O35" s="75"/>
-      <c r="P35" s="75"/>
-      <c r="Q35" s="73"/>
-      <c r="R35" s="77"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="37"/>
+      <c r="O35" s="37"/>
+      <c r="P35" s="37"/>
+      <c r="Q35" s="37"/>
+      <c r="R35" s="37"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
-      <c r="B36" s="29"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="31"/>
-      <c r="L36" s="31"/>
-      <c r="M36" s="32"/>
-      <c r="N36" s="32"/>
-      <c r="O36" s="32"/>
-      <c r="P36" s="32"/>
-      <c r="Q36" s="32"/>
-      <c r="R36" s="32"/>
+      <c r="A36" s="38"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="36"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B37" s="66" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" s="66"/>
-      <c r="D37" s="66"/>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
-      <c r="G37" s="66"/>
-      <c r="H37" s="66"/>
-      <c r="I37" s="66"/>
-      <c r="J37" s="66"/>
-      <c r="K37" s="66"/>
-      <c r="L37" s="66"/>
-      <c r="M37" s="66"/>
-      <c r="N37" s="66"/>
-      <c r="O37" s="66"/>
-      <c r="P37" s="66"/>
-      <c r="Q37" s="66"/>
-      <c r="R37" s="66"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="68"/>
+      <c r="C37" s="68"/>
+      <c r="D37" s="68"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="41"/>
+      <c r="H37" s="41"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
-      <c r="B38" s="66" t="s">
-        <v>52</v>
-      </c>
-      <c r="C38" s="66"/>
-      <c r="D38" s="66"/>
-      <c r="E38" s="66"/>
-      <c r="F38" s="66"/>
-      <c r="G38" s="66"/>
-      <c r="H38" s="66"/>
-      <c r="I38" s="66"/>
-      <c r="J38" s="66"/>
-      <c r="K38" s="66"/>
-      <c r="L38" s="66"/>
-      <c r="M38" s="66"/>
-      <c r="N38" s="66"/>
-      <c r="O38" s="66"/>
-      <c r="P38" s="66"/>
-      <c r="Q38" s="66"/>
-      <c r="R38" s="66"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="36"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
-      <c r="B39" s="66" t="s">
-        <v>53</v>
-      </c>
-      <c r="C39" s="66"/>
-      <c r="D39" s="66"/>
-      <c r="E39" s="66"/>
-      <c r="F39" s="66"/>
-      <c r="G39" s="66"/>
-      <c r="H39" s="66"/>
-      <c r="I39" s="66"/>
-      <c r="J39" s="66"/>
-      <c r="K39" s="66"/>
-      <c r="L39" s="66"/>
-      <c r="M39" s="66"/>
-      <c r="N39" s="66"/>
-      <c r="O39" s="66"/>
-      <c r="P39" s="66"/>
-      <c r="Q39" s="66"/>
-      <c r="R39" s="66"/>
+      <c r="A39" s="42"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="41"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
-      <c r="B40" s="66" t="s">
-        <v>54</v>
-      </c>
-      <c r="C40" s="66"/>
-      <c r="D40" s="66"/>
-      <c r="E40" s="66"/>
-      <c r="F40" s="66"/>
-      <c r="G40" s="66"/>
-      <c r="H40" s="66"/>
-      <c r="I40" s="66"/>
-      <c r="J40" s="66"/>
-      <c r="K40" s="66"/>
-      <c r="L40" s="66"/>
-      <c r="M40" s="66"/>
-      <c r="N40" s="66"/>
-      <c r="O40" s="66"/>
-      <c r="P40" s="66"/>
-      <c r="Q40" s="66"/>
-      <c r="R40" s="66"/>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="33"/>
-      <c r="B41" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="C41" s="35"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="37"/>
-      <c r="I41" s="38"/>
-      <c r="J41" s="38"/>
-      <c r="K41" s="38"/>
-      <c r="L41" s="38"/>
-      <c r="M41" s="38"/>
-      <c r="N41" s="38"/>
-      <c r="O41" s="38"/>
-      <c r="P41" s="38"/>
-      <c r="Q41" s="38"/>
-      <c r="R41" s="38"/>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="39"/>
-      <c r="B42" s="40"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="33"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="37"/>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="41"/>
-      <c r="B43" s="63"/>
-      <c r="C43" s="63"/>
-      <c r="D43" s="63"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="42"/>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="41"/>
-      <c r="B44" s="40"/>
-      <c r="C44" s="40"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="33"/>
-      <c r="H44" s="37"/>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="43"/>
-      <c r="B45" s="40"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="42"/>
-      <c r="G45" s="42"/>
-      <c r="H45" s="42"/>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="41"/>
-      <c r="B46" s="41"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="37"/>
-      <c r="G46" s="37"/>
-      <c r="H46" s="37"/>
+      <c r="A40" s="40"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B37:D37"/>
     <mergeCell ref="P14:P15"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="B37:R37"/>
-    <mergeCell ref="B38:R38"/>
-    <mergeCell ref="B39:R39"/>
-    <mergeCell ref="B40:R40"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="B31:R31"/>
+    <mergeCell ref="B32:R32"/>
+    <mergeCell ref="B33:R33"/>
+    <mergeCell ref="B34:R34"/>
     <mergeCell ref="Q13:Q15"/>
     <mergeCell ref="R13:R15"/>
     <mergeCell ref="D14:D15"/>

</xml_diff>